<commit_message>
Update files based on cn190115 and Improve Translation for console
</commit_message>
<xml_diff>
--- a/console/Networking/iaas网络与容器中文提取/subnetExcel/detail.xlsx
+++ b/console/Networking/iaas网络与容器中文提取/subnetExcel/detail.xlsx
@@ -5,16 +5,16 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\韩凯\2019.1\console;Networking;iaas网络与容器中文提取-0107-译文-提交\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\文件\工作-中译语通\2018年\12月\12月4日\VPC和子网国际化-by-JD\最终版\subnetExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="ch" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -473,18 +473,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>所属网络</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>detail_i18nKey_20</t>
     </r>
   </si>
@@ -569,18 +557,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>当前绑定路由表</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>detail_i18nKey_24</t>
     </r>
   </si>
@@ -641,18 +617,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">此子网未绑定ACL规则 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>detail_i18nKey_27</t>
     </r>
   </si>
@@ -689,18 +653,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>当前绑定ACL</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>detail_i18nKey_29</t>
     </r>
   </si>
@@ -1385,18 +1337,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Hosting VPC</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>'Available IPv4'</t>
     </r>
   </si>
@@ -1433,18 +1373,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Currently-Associated Route Table</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Change Route Table</t>
     </r>
   </si>
@@ -1469,18 +1397,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">ACL rules are not associated with the subnet </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Associate</t>
     </r>
   </si>
@@ -1493,18 +1409,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Currently-Associated ACL</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Disassociated</t>
     </r>
   </si>
@@ -1637,18 +1541,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Name only supports Chinese, numbers, upper case and lower case letters, English underline “_” and line-through</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Description length cannot exceed 256 characters</t>
     </r>
   </si>
@@ -1661,18 +1553,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Description only supports Chinese, numbers, upper case and lower case letters and English underline “_”</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>'Disassociate ACL'</t>
     </r>
   </si>
@@ -1686,30 +1566,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>'Your subnet will lose security protection after disassociation</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Confirm to delete the subnet</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'Delete subnet'</t>
     </r>
   </si>
   <si>
@@ -1721,15 +1577,214 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Change route table'</t>
+    <t>VPC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Name only supports </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chinese characters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, numbers, upper case and lower case letters, English underline “_” and line-through</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Description only supports </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chinese characters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, numbers, upper case and lower case letters and English underline “_”</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Associated Route Table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Associated ACL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Confirm to delete the</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Subnet</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Delete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Subnet'</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Change </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Route Table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所属网络</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前绑定路由表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>此子网未绑定</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ACL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>规则</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>当前绑定</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ACL</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">No ACL rule is  associated with the Subnet </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1739,6 +1794,21 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1765,12 +1835,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2112,10 +2188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="B52" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2133,7 +2209,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2144,7 +2220,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2155,7 +2231,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2166,7 +2242,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2177,7 +2253,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2188,7 +2264,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2199,7 +2275,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2210,7 +2286,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2221,7 +2297,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2232,7 +2308,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2243,7 +2319,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2254,7 +2330,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2265,7 +2341,7 @@
         <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2276,7 +2352,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.2">
@@ -2287,7 +2363,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2298,10 +2374,10 @@
         <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -2309,10 +2385,10 @@
         <v>33</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -2320,344 +2396,364 @@
         <v>35</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="1" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="1" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="1" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="1" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="1" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="1" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="1" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="1" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="1" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="1" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="1" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="1" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="1" t="s">
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="1" t="s">
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="1" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" s="1" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>140</v>
-      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:B48" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:B18 A20:B22 A19 A24:B25 A23 A27:B27 A26 A29:B48 A28" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>